<commit_message>
changed tarif to june
</commit_message>
<xml_diff>
--- a/bsd_tarif.xlsx
+++ b/bsd_tarif.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF799E3-8E19-4924-9B62-AECB6FB48AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26860527-A46B-4CBB-A3BF-B25CB7DE2D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t xml:space="preserve">Город отправления </t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Ростов-на-Дону</t>
-  </si>
-  <si>
-    <t>Луганск/ Стаханова/ Алчевск</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -404,12 +401,6 @@
     <t>Петровское</t>
   </si>
   <si>
-    <t>Горловка/ Енакиево/ Шахтерск</t>
-  </si>
-  <si>
-    <t>Снежное / Кр Луч</t>
-  </si>
-  <si>
     <t>до 2 кг</t>
   </si>
   <si>
@@ -569,10 +560,25 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Макеевка/  Донецк </t>
+    <t xml:space="preserve">Донецк </t>
   </si>
   <si>
-    <t>Бердянск / Мелитолполь</t>
+    <t xml:space="preserve">Горловка/ Енакиево/ </t>
+  </si>
+  <si>
+    <t>Шахтерск/ Снежное / Кр Луч</t>
+  </si>
+  <si>
+    <t>Луганск</t>
+  </si>
+  <si>
+    <t>Стаханова/ Алчевск</t>
+  </si>
+  <si>
+    <t>Бердянск , Мелитолполь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Макеевка, </t>
   </si>
 </sst>
 </file>
@@ -9891,7 +9897,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -10064,11 +10070,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -10100,68 +10158,22 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -19210,457 +19222,559 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="97" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="97" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" style="97" customWidth="1"/>
-    <col min="4" max="17" width="11.7109375" style="95" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="95"/>
+    <col min="1" max="1" width="16.85546875" style="75" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="75" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" style="75" customWidth="1"/>
+    <col min="4" max="17" width="11.7109375" style="74" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="85" t="s">
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="85" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="86" t="s">
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="86" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="86" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="86" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" s="86" t="s">
+      <c r="N2" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="M2" s="86" t="s">
+      <c r="P2" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="86" t="s">
+      <c r="Q2" s="67" t="s">
         <v>73</v>
-      </c>
-      <c r="O2" s="86" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" s="86" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q2" s="86" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="83"/>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="89">
-        <v>0</v>
-      </c>
-      <c r="E3" s="90">
+      <c r="A3" s="66"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="69">
+        <v>0</v>
+      </c>
+      <c r="E3" s="70">
         <v>1</v>
       </c>
-      <c r="F3" s="90">
+      <c r="F3" s="70">
         <v>2</v>
       </c>
-      <c r="G3" s="89">
+      <c r="G3" s="69">
         <v>3</v>
       </c>
-      <c r="H3" s="90">
+      <c r="H3" s="70">
         <v>4</v>
       </c>
-      <c r="I3" s="90">
+      <c r="I3" s="70">
         <v>5</v>
       </c>
-      <c r="J3" s="89">
+      <c r="J3" s="69">
         <v>6</v>
       </c>
-      <c r="K3" s="91">
+      <c r="K3" s="71">
         <v>7</v>
       </c>
-      <c r="L3" s="91">
+      <c r="L3" s="71">
         <v>8</v>
       </c>
-      <c r="M3" s="92">
+      <c r="M3" s="72">
         <v>9</v>
       </c>
-      <c r="N3" s="91">
+      <c r="N3" s="71">
         <v>10</v>
       </c>
-      <c r="O3" s="91">
+      <c r="O3" s="71">
         <v>11</v>
       </c>
-      <c r="P3" s="92">
+      <c r="P3" s="72">
         <v>12</v>
       </c>
-      <c r="Q3" s="91">
+      <c r="Q3" s="71">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="81" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="93">
-        <v>0</v>
-      </c>
-      <c r="D4" s="94">
-        <v>650</v>
-      </c>
-      <c r="E4" s="94">
-        <v>26</v>
-      </c>
-      <c r="F4" s="96">
+      <c r="B4" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="73">
+        <v>0</v>
+      </c>
+      <c r="D4" s="96">
+        <v>600</v>
+      </c>
+      <c r="E4" s="96">
+        <v>34</v>
+      </c>
+      <c r="F4" s="97">
+        <v>20</v>
+      </c>
+      <c r="G4" s="97">
+        <v>20</v>
+      </c>
+      <c r="H4" s="97">
         <v>19</v>
       </c>
-      <c r="G4" s="96">
+      <c r="I4" s="97">
         <v>18</v>
       </c>
-      <c r="H4" s="96">
-        <v>17</v>
-      </c>
-      <c r="I4" s="96">
-        <v>17</v>
-      </c>
-      <c r="J4" s="96">
-        <v>16</v>
-      </c>
-      <c r="K4" s="94">
-        <v>650</v>
-      </c>
-      <c r="L4" s="94">
-        <v>6500</v>
-      </c>
-      <c r="M4" s="94">
+      <c r="J4" s="97">
+        <v>18</v>
+      </c>
+      <c r="K4" s="96">
+        <v>600</v>
+      </c>
+      <c r="L4" s="96">
+        <v>8500</v>
+      </c>
+      <c r="M4" s="96">
+        <v>5000</v>
+      </c>
+      <c r="N4" s="96">
+        <v>5000</v>
+      </c>
+      <c r="O4" s="96">
         <v>4750</v>
       </c>
-      <c r="N4" s="94">
+      <c r="P4" s="96">
         <v>4500</v>
       </c>
-      <c r="O4" s="94">
-        <v>4250</v>
-      </c>
-      <c r="P4" s="94">
-        <v>4250</v>
-      </c>
-      <c r="Q4" s="94">
-        <v>4000</v>
+      <c r="Q4" s="96">
+        <v>4500</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="84"/>
-      <c r="B5" s="82" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="93">
+      <c r="A5" s="95"/>
+      <c r="B5" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="73">
         <v>1</v>
       </c>
-      <c r="D5" s="94">
-        <v>650</v>
-      </c>
-      <c r="E5" s="94">
-        <v>26</v>
-      </c>
-      <c r="F5" s="96">
-        <v>19</v>
-      </c>
-      <c r="G5" s="96">
+      <c r="D5" s="96">
+        <v>600</v>
+      </c>
+      <c r="E5" s="96">
+        <v>30</v>
+      </c>
+      <c r="F5" s="97">
         <v>18</v>
       </c>
-      <c r="H5" s="96">
+      <c r="G5" s="97">
         <v>17</v>
       </c>
-      <c r="I5" s="96">
+      <c r="H5" s="97">
         <v>17</v>
       </c>
-      <c r="J5" s="96">
+      <c r="I5" s="97">
         <v>16</v>
       </c>
-      <c r="K5" s="94">
-        <v>650</v>
-      </c>
-      <c r="L5" s="94">
-        <v>6500</v>
-      </c>
-      <c r="M5" s="94">
-        <v>4750</v>
-      </c>
-      <c r="N5" s="94">
+      <c r="J5" s="97">
+        <v>16</v>
+      </c>
+      <c r="K5" s="96">
+        <v>600</v>
+      </c>
+      <c r="L5" s="96">
+        <v>7500</v>
+      </c>
+      <c r="M5" s="96">
         <v>4500</v>
       </c>
-      <c r="O5" s="94">
+      <c r="N5" s="96">
         <v>4250</v>
       </c>
-      <c r="P5" s="94">
+      <c r="O5" s="96">
         <v>4250</v>
       </c>
-      <c r="Q5" s="94">
+      <c r="P5" s="96">
+        <v>4000</v>
+      </c>
+      <c r="Q5" s="96">
         <v>4000</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
-      <c r="B6" s="82" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="93">
+      <c r="A6" s="95"/>
+      <c r="B6" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="73">
         <v>2</v>
       </c>
-      <c r="D6" s="94">
-        <v>650</v>
-      </c>
-      <c r="E6" s="94">
-        <v>26</v>
-      </c>
-      <c r="F6" s="96">
+      <c r="D6" s="96">
+        <v>600</v>
+      </c>
+      <c r="E6" s="96">
+        <v>34</v>
+      </c>
+      <c r="F6" s="97">
+        <v>20</v>
+      </c>
+      <c r="G6" s="97">
+        <v>20</v>
+      </c>
+      <c r="H6" s="97">
         <v>19</v>
       </c>
-      <c r="G6" s="96">
+      <c r="I6" s="97">
         <v>18</v>
       </c>
-      <c r="H6" s="96">
-        <v>17</v>
-      </c>
-      <c r="I6" s="96">
-        <v>17</v>
-      </c>
-      <c r="J6" s="96">
-        <v>16</v>
-      </c>
-      <c r="K6" s="94">
-        <v>650</v>
-      </c>
-      <c r="L6" s="94">
-        <v>6500</v>
-      </c>
-      <c r="M6" s="94">
+      <c r="J6" s="97">
+        <v>18</v>
+      </c>
+      <c r="K6" s="96">
+        <v>600</v>
+      </c>
+      <c r="L6" s="96">
+        <v>8500</v>
+      </c>
+      <c r="M6" s="96">
+        <v>5000</v>
+      </c>
+      <c r="N6" s="96">
+        <v>5000</v>
+      </c>
+      <c r="O6" s="96">
         <v>4750</v>
       </c>
-      <c r="N6" s="94">
+      <c r="P6" s="96">
         <v>4500</v>
       </c>
-      <c r="O6" s="94">
-        <v>4250</v>
-      </c>
-      <c r="P6" s="94">
-        <v>4250</v>
-      </c>
-      <c r="Q6" s="94">
-        <v>4000</v>
+      <c r="Q6" s="96">
+        <v>4500</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
-      <c r="B7" s="82" t="s">
+      <c r="A7" s="95"/>
+      <c r="B7" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="73">
+        <v>3</v>
+      </c>
+      <c r="D7" s="96">
+        <v>600</v>
+      </c>
+      <c r="E7" s="96">
+        <v>34</v>
+      </c>
+      <c r="F7" s="97">
+        <v>20</v>
+      </c>
+      <c r="G7" s="97">
+        <v>20</v>
+      </c>
+      <c r="H7" s="97">
         <v>19</v>
       </c>
-      <c r="C7" s="93">
-        <v>3</v>
-      </c>
-      <c r="D7" s="94">
-        <v>650</v>
-      </c>
-      <c r="E7" s="94">
-        <v>26</v>
-      </c>
-      <c r="F7" s="96">
-        <v>19</v>
-      </c>
-      <c r="G7" s="96">
-        <v>18</v>
-      </c>
-      <c r="H7" s="96">
+      <c r="I7" s="97">
         <v>17</v>
       </c>
-      <c r="I7" s="96">
-        <v>17</v>
-      </c>
-      <c r="J7" s="96">
+      <c r="J7" s="97">
         <v>16</v>
       </c>
-      <c r="K7" s="94">
-        <v>650</v>
-      </c>
-      <c r="L7" s="94">
-        <v>6500</v>
-      </c>
-      <c r="M7" s="94">
+      <c r="K7" s="96">
+        <v>600</v>
+      </c>
+      <c r="L7" s="96">
+        <v>8500</v>
+      </c>
+      <c r="M7" s="96">
+        <v>5000</v>
+      </c>
+      <c r="N7" s="96">
+        <v>5000</v>
+      </c>
+      <c r="O7" s="96">
         <v>4750</v>
       </c>
-      <c r="N7" s="94">
-        <v>4500</v>
-      </c>
-      <c r="O7" s="94">
+      <c r="P7" s="96">
         <v>4250</v>
       </c>
-      <c r="P7" s="94">
-        <v>4250</v>
-      </c>
-      <c r="Q7" s="94">
+      <c r="Q7" s="96">
         <v>4000</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="84"/>
-      <c r="B8" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="93">
+      <c r="A8" s="95"/>
+      <c r="B8" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="73">
         <v>4</v>
       </c>
-      <c r="D8" s="94">
-        <v>650</v>
-      </c>
-      <c r="E8" s="94">
-        <v>26</v>
-      </c>
-      <c r="F8" s="96">
-        <v>19</v>
-      </c>
-      <c r="G8" s="96">
+      <c r="D8" s="96">
+        <v>600</v>
+      </c>
+      <c r="E8" s="96">
+        <v>30</v>
+      </c>
+      <c r="F8" s="97">
         <v>18</v>
       </c>
-      <c r="H8" s="96">
+      <c r="G8" s="97">
         <v>17</v>
       </c>
-      <c r="I8" s="96">
+      <c r="H8" s="97">
         <v>17</v>
       </c>
-      <c r="J8" s="96">
+      <c r="I8" s="97">
         <v>16</v>
       </c>
-      <c r="K8" s="94">
-        <v>650</v>
-      </c>
-      <c r="L8" s="94">
-        <v>6500</v>
-      </c>
-      <c r="M8" s="94">
-        <v>4750</v>
-      </c>
-      <c r="N8" s="94">
+      <c r="J8" s="97">
+        <v>16</v>
+      </c>
+      <c r="K8" s="96">
+        <v>600</v>
+      </c>
+      <c r="L8" s="96">
+        <v>7500</v>
+      </c>
+      <c r="M8" s="96">
         <v>4500</v>
       </c>
-      <c r="O8" s="94">
+      <c r="N8" s="96">
         <v>4250</v>
       </c>
-      <c r="P8" s="94">
+      <c r="O8" s="96">
         <v>4250</v>
       </c>
-      <c r="Q8" s="94">
+      <c r="P8" s="96">
+        <v>4000</v>
+      </c>
+      <c r="Q8" s="96">
         <v>4000</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
-      <c r="B9" s="81" t="s">
+      <c r="A9" s="95"/>
+      <c r="B9" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="93">
+      <c r="C9" s="73">
         <v>5</v>
       </c>
-      <c r="D9" s="94">
+      <c r="D9" s="96">
+        <v>600</v>
+      </c>
+      <c r="E9" s="96">
+        <v>34</v>
+      </c>
+      <c r="F9" s="97">
+        <v>20</v>
+      </c>
+      <c r="G9" s="97">
+        <v>20</v>
+      </c>
+      <c r="H9" s="97">
+        <v>19</v>
+      </c>
+      <c r="I9" s="97">
+        <v>18</v>
+      </c>
+      <c r="J9" s="97">
+        <v>18</v>
+      </c>
+      <c r="K9" s="96">
+        <v>600</v>
+      </c>
+      <c r="L9" s="96">
+        <v>8500</v>
+      </c>
+      <c r="M9" s="96">
+        <v>5000</v>
+      </c>
+      <c r="N9" s="96">
+        <v>5000</v>
+      </c>
+      <c r="O9" s="96">
+        <v>4750</v>
+      </c>
+      <c r="P9" s="96">
+        <v>4500</v>
+      </c>
+      <c r="Q9" s="96">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="95"/>
+      <c r="B10" s="99" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="73">
+        <v>6</v>
+      </c>
+      <c r="D10" s="98">
+        <v>600</v>
+      </c>
+      <c r="E10" s="98">
+        <v>36</v>
+      </c>
+      <c r="F10" s="98">
+        <v>20</v>
+      </c>
+      <c r="G10" s="98">
+        <v>20</v>
+      </c>
+      <c r="H10" s="98">
+        <v>19</v>
+      </c>
+      <c r="I10" s="98">
+        <v>17</v>
+      </c>
+      <c r="J10" s="98">
+        <v>16</v>
+      </c>
+      <c r="K10" s="98">
+        <v>600</v>
+      </c>
+      <c r="L10" s="98">
+        <v>9000</v>
+      </c>
+      <c r="M10" s="98">
+        <v>5000</v>
+      </c>
+      <c r="N10" s="98">
+        <v>5000</v>
+      </c>
+      <c r="O10" s="98">
+        <v>4750</v>
+      </c>
+      <c r="P10" s="98">
+        <v>4250</v>
+      </c>
+      <c r="Q10" s="98">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="95"/>
+      <c r="B11" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="73">
+        <v>7</v>
+      </c>
+      <c r="D11" s="98">
         <v>700</v>
       </c>
-      <c r="E9" s="94">
-        <v>32</v>
-      </c>
-      <c r="F9" s="96">
-        <v>24</v>
-      </c>
-      <c r="G9" s="96">
+      <c r="E11" s="98">
+        <v>44</v>
+      </c>
+      <c r="F11" s="98">
+        <v>28</v>
+      </c>
+      <c r="G11" s="98">
+        <v>28</v>
+      </c>
+      <c r="H11" s="98">
+        <v>26</v>
+      </c>
+      <c r="I11" s="98">
         <v>23</v>
       </c>
-      <c r="H9" s="96">
-        <v>21</v>
-      </c>
-      <c r="I9" s="96">
-        <v>21</v>
-      </c>
-      <c r="J9" s="96">
-        <v>20</v>
-      </c>
-      <c r="K9" s="94">
+      <c r="J11" s="98">
+        <v>22</v>
+      </c>
+      <c r="K11" s="98">
         <v>700</v>
       </c>
-      <c r="L9" s="94">
-        <v>8000</v>
-      </c>
-      <c r="M9" s="94">
-        <v>6000</v>
-      </c>
-      <c r="N9" s="94">
+      <c r="L11" s="98">
+        <v>11000</v>
+      </c>
+      <c r="M11" s="98">
+        <v>7000</v>
+      </c>
+      <c r="N11" s="98">
+        <v>7000</v>
+      </c>
+      <c r="O11" s="98">
+        <v>6500</v>
+      </c>
+      <c r="P11" s="98">
         <v>5750</v>
       </c>
-      <c r="O9" s="94">
-        <v>5250</v>
-      </c>
-      <c r="P9" s="94">
-        <v>5250</v>
-      </c>
-      <c r="Q9" s="94">
-        <v>5000</v>
+      <c r="Q11" s="98">
+        <v>5500</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A4:A9"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="K1:Q1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A4:A11"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
@@ -19687,12 +19801,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="6" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="80"/>
+      <c r="A1" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="83"/>
       <c r="E1" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -19711,42 +19825,42 @@
       <c r="T1" s="7"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="81" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="64" t="s">
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
     </row>
     <row r="3" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="77"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="79"/>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
@@ -19792,10 +19906,10 @@
     </row>
     <row r="4" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="73" t="s">
-        <v>26</v>
+        <v>54</v>
+      </c>
+      <c r="B4" s="91" t="s">
+        <v>25</v>
       </c>
       <c r="C4" s="20">
         <v>300</v>
@@ -19851,9 +19965,9 @@
     </row>
     <row r="5" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="74"/>
+        <v>30</v>
+      </c>
+      <c r="B5" s="92"/>
       <c r="C5" s="8">
         <v>300</v>
       </c>
@@ -19908,9 +20022,9 @@
     </row>
     <row r="6" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="74"/>
+        <v>26</v>
+      </c>
+      <c r="B6" s="92"/>
       <c r="C6" s="10">
         <v>350</v>
       </c>
@@ -19965,9 +20079,9 @@
     </row>
     <row r="7" spans="1:20" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="74"/>
+        <v>27</v>
+      </c>
+      <c r="B7" s="92"/>
       <c r="C7" s="12">
         <v>350</v>
       </c>
@@ -20022,9 +20136,9 @@
     </row>
     <row r="8" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="74"/>
+        <v>28</v>
+      </c>
+      <c r="B8" s="92"/>
       <c r="C8" s="10">
         <v>350</v>
       </c>
@@ -20079,9 +20193,9 @@
     </row>
     <row r="9" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="74"/>
+        <v>29</v>
+      </c>
+      <c r="B9" s="92"/>
       <c r="C9" s="10">
         <v>350</v>
       </c>
@@ -20136,9 +20250,9 @@
     </row>
     <row r="10" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="74"/>
+        <v>55</v>
+      </c>
+      <c r="B10" s="92"/>
       <c r="C10" s="10">
         <v>400</v>
       </c>
@@ -20193,9 +20307,9 @@
     </row>
     <row r="11" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="74"/>
+        <v>31</v>
+      </c>
+      <c r="B11" s="92"/>
       <c r="C11" s="10">
         <v>400</v>
       </c>
@@ -20250,9 +20364,9 @@
     </row>
     <row r="12" spans="1:20" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="74"/>
+        <v>32</v>
+      </c>
+      <c r="B12" s="92"/>
       <c r="C12" s="12">
         <v>350</v>
       </c>
@@ -20307,9 +20421,9 @@
     </row>
     <row r="13" spans="1:20" s="9" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="74"/>
+        <v>33</v>
+      </c>
+      <c r="B13" s="92"/>
       <c r="C13" s="12">
         <v>350</v>
       </c>
@@ -20364,9 +20478,9 @@
     </row>
     <row r="14" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="74"/>
+        <v>34</v>
+      </c>
+      <c r="B14" s="92"/>
       <c r="C14" s="12">
         <v>350</v>
       </c>
@@ -20421,9 +20535,9 @@
     </row>
     <row r="15" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="74"/>
+        <v>35</v>
+      </c>
+      <c r="B15" s="92"/>
       <c r="C15" s="12">
         <v>350</v>
       </c>
@@ -20478,9 +20592,9 @@
     </row>
     <row r="16" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="74"/>
+        <v>36</v>
+      </c>
+      <c r="B16" s="92"/>
       <c r="C16" s="12">
         <v>350</v>
       </c>
@@ -20535,9 +20649,9 @@
     </row>
     <row r="17" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="74"/>
+        <v>37</v>
+      </c>
+      <c r="B17" s="92"/>
       <c r="C17" s="12">
         <v>300</v>
       </c>
@@ -20592,9 +20706,9 @@
     </row>
     <row r="18" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="74"/>
+        <v>38</v>
+      </c>
+      <c r="B18" s="92"/>
       <c r="C18" s="12">
         <v>300</v>
       </c>
@@ -20649,9 +20763,9 @@
     </row>
     <row r="19" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="74"/>
+        <v>39</v>
+      </c>
+      <c r="B19" s="92"/>
       <c r="C19" s="12">
         <v>350</v>
       </c>
@@ -20706,9 +20820,9 @@
     </row>
     <row r="20" spans="1:18" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="75"/>
+        <v>40</v>
+      </c>
+      <c r="B20" s="93"/>
       <c r="C20" s="30">
         <v>350</v>
       </c>
@@ -20763,10 +20877,10 @@
     </row>
     <row r="21" spans="1:18" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="89" t="s">
         <v>42</v>
-      </c>
-      <c r="B21" s="71" t="s">
-        <v>43</v>
       </c>
       <c r="C21" s="37">
         <v>300</v>
@@ -20822,9 +20936,9 @@
     </row>
     <row r="22" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="69"/>
+        <v>43</v>
+      </c>
+      <c r="B22" s="87"/>
       <c r="C22" s="14">
         <v>300</v>
       </c>
@@ -20879,9 +20993,9 @@
     </row>
     <row r="23" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="69"/>
+        <v>44</v>
+      </c>
+      <c r="B23" s="87"/>
       <c r="C23" s="14">
         <v>300</v>
       </c>
@@ -20936,9 +21050,9 @@
     </row>
     <row r="24" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="69"/>
+        <v>45</v>
+      </c>
+      <c r="B24" s="87"/>
       <c r="C24" s="35">
         <v>400</v>
       </c>
@@ -20993,9 +21107,9 @@
     </row>
     <row r="25" spans="1:18" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="72"/>
+        <v>46</v>
+      </c>
+      <c r="B25" s="90"/>
       <c r="C25" s="40">
         <v>400</v>
       </c>
@@ -21050,16 +21164,16 @@
     </row>
     <row r="26" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="68" t="s">
-        <v>35</v>
+        <v>65</v>
+      </c>
+      <c r="B26" s="86" t="s">
+        <v>34</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="61">
         <v>1600</v>
@@ -21108,9 +21222,9 @@
     </row>
     <row r="27" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="69"/>
+        <v>34</v>
+      </c>
+      <c r="B27" s="87"/>
       <c r="C27" s="8">
         <v>300</v>
       </c>
@@ -21165,14 +21279,14 @@
     </row>
     <row r="28" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="69"/>
+        <v>48</v>
+      </c>
+      <c r="B28" s="87"/>
       <c r="C28" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="35">
         <v>1600</v>
@@ -21221,14 +21335,14 @@
     </row>
     <row r="29" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="69"/>
+        <v>49</v>
+      </c>
+      <c r="B29" s="87"/>
       <c r="C29" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="35">
         <v>1600</v>
@@ -21277,14 +21391,14 @@
     </row>
     <row r="30" spans="1:18" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="70"/>
+        <v>50</v>
+      </c>
+      <c r="B30" s="88"/>
       <c r="C30" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="54">
         <v>1400</v>
@@ -21333,10 +21447,10 @@
     </row>
     <row r="31" spans="1:18" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="71" t="s">
-        <v>52</v>
+        <v>64</v>
+      </c>
+      <c r="B31" s="89" t="s">
+        <v>51</v>
       </c>
       <c r="C31" s="37">
         <v>300</v>
@@ -21392,9 +21506,9 @@
     </row>
     <row r="32" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="69"/>
+        <v>63</v>
+      </c>
+      <c r="B32" s="87"/>
       <c r="C32" s="14">
         <v>300</v>
       </c>
@@ -21449,9 +21563,9 @@
     </row>
     <row r="33" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="69"/>
+        <v>52</v>
+      </c>
+      <c r="B33" s="87"/>
       <c r="C33" s="14">
         <v>350</v>
       </c>
@@ -21506,9 +21620,9 @@
     </row>
     <row r="34" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="B34" s="87"/>
       <c r="C34" s="14">
         <v>400</v>
       </c>
@@ -21563,9 +21677,9 @@
     </row>
     <row r="35" spans="1:18" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="72"/>
+        <v>53</v>
+      </c>
+      <c r="B35" s="90"/>
       <c r="C35" s="43">
         <v>350</v>
       </c>
@@ -21667,10 +21781,10 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
@@ -21702,7 +21816,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
@@ -21719,7 +21833,7 @@
     </row>
     <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
@@ -22072,17 +22186,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B4:B20"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:K2"/>
     <mergeCell ref="L2:R2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B4:B20"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId1"/>

</xml_diff>